<commit_message>
Processed more fecundity data
</commit_message>
<xml_diff>
--- a/Data_Moities/Fecundity.xlsx
+++ b/Data_Moities/Fecundity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardhonor/Documents/R/masters_thesis/Synthesis/Data_Moities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0C3914-BBE3-B44E-9BB1-952A6C3137C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F0F73C-D905-5647-9628-C8BC1DD0E44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{3BBC4001-F2E5-6945-A434-591B9071637E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="254">
   <si>
     <t>Tag</t>
   </si>
@@ -471,16 +471,346 @@
   </si>
   <si>
     <t xml:space="preserve">possible error -- no label in bag but only one left.  </t>
+  </si>
+  <si>
+    <t>d§JBCHY1/1/50§Q§273</t>
+  </si>
+  <si>
+    <t>b§KVEDG1/1/80§Q§279</t>
+  </si>
+  <si>
+    <t>e§VRCAN/1/40§Q§504</t>
+  </si>
+  <si>
+    <t>b§WSSWM3/1/0§Q§569</t>
+  </si>
+  <si>
+    <t>b§JBCHY1/1/50§Q§227</t>
+  </si>
+  <si>
+    <t>a§DVGM/20§Q§105</t>
+  </si>
+  <si>
+    <t>a§KVEDG1/1/80§Q§275</t>
+  </si>
+  <si>
+    <t>a§DVGM/20§Q§107</t>
+  </si>
+  <si>
+    <t>d§CRSOSO/3/40§Q§62</t>
+  </si>
+  <si>
+    <t>d§CBMCK1/3/60§N§i115</t>
+  </si>
+  <si>
+    <t>d§KVEDG1/1/80§Q§294</t>
+  </si>
+  <si>
+    <t>c§CBMCK1/1/0§N§42</t>
+  </si>
+  <si>
+    <t>d§VRCAN/1/40§Q§501</t>
+  </si>
+  <si>
+    <t>d§JARI1/1/80§Q§180</t>
+  </si>
+  <si>
+    <t>b§JBCHY1/1/50§Q§242</t>
+  </si>
+  <si>
+    <t>b§MHBUR1/4/20§Q§343</t>
+  </si>
+  <si>
+    <t>c§CWRIC2/X2§Q§91</t>
+  </si>
+  <si>
+    <t>c§JBBLB2/1/20§Q§210</t>
+  </si>
+  <si>
+    <t>c§VRCAN/1/40§Q§491</t>
+  </si>
+  <si>
+    <t>d§JARI1/1/80§Q§184</t>
+  </si>
+  <si>
+    <t>a§SMITH1/20§Q§456</t>
+  </si>
+  <si>
+    <t>b§VRPET2/3/20§Q§510</t>
+  </si>
+  <si>
+    <t>maple/cnt§11</t>
+  </si>
+  <si>
+    <t>a§VSGARO1/1/0§Q§533</t>
+  </si>
+  <si>
+    <t>d§MHBUR1/4/20§Q§350</t>
+  </si>
+  <si>
+    <t>e§RULEB1/20§N§429</t>
+  </si>
+  <si>
+    <t>e§WSSWM3/1/0§Q§575</t>
+  </si>
+  <si>
+    <t>maple/cnt§27</t>
+  </si>
+  <si>
+    <t>maple/cnt§15</t>
+  </si>
+  <si>
+    <t>a§CBMCK1/1/0§N§36</t>
+  </si>
+  <si>
+    <t>c§CWRIC2/X2§Q§92</t>
+  </si>
+  <si>
+    <t>b§VRCAN/1/40§Q§482</t>
+  </si>
+  <si>
+    <t>d§CWRIC2/X2§Q§98</t>
+  </si>
+  <si>
+    <t>b§SMITH1/20§Q§464</t>
+  </si>
+  <si>
+    <t>d§JWBOY/2/80§Q§262</t>
+  </si>
+  <si>
+    <t>e§EFCC2/4/80§Q§157</t>
+  </si>
+  <si>
+    <t>d§CWRIC2/X2§Q§96</t>
+  </si>
+  <si>
+    <t>a§CBMCK1/1/0§N§35</t>
+  </si>
+  <si>
+    <t>d§DVGM/20§Q§122</t>
+  </si>
+  <si>
+    <t>d§MSMID1/1/20§Q§392</t>
+  </si>
+  <si>
+    <t>a§WSSWM3/1/0§Q§555</t>
+  </si>
+  <si>
+    <t>a§SMAKC1/B§N§432</t>
+  </si>
+  <si>
+    <t>d§MAVBEL2/1/20§N§325</t>
+  </si>
+  <si>
+    <t>b§EFCC2/4/80§Q§144</t>
+  </si>
+  <si>
+    <t>c§MHBUR1/4/20§Q§344</t>
+  </si>
+  <si>
+    <t>d§VRPET2/3/20§Q§506</t>
+  </si>
+  <si>
+    <t>b§JARI1/1/80§Q§172</t>
+  </si>
+  <si>
+    <t>e§WSSWM3/1/0§Q§573</t>
+  </si>
+  <si>
+    <t>e§MAVBEL2/1/20§N§329</t>
+  </si>
+  <si>
+    <t>b§JBBLB2/1/20§Q§202</t>
+  </si>
+  <si>
+    <t>maple/cnt§14</t>
+  </si>
+  <si>
+    <t>e§PDVRT1/20§Q§418</t>
+  </si>
+  <si>
+    <t>b§MHNAT1/2/0§Q§358</t>
+  </si>
+  <si>
+    <t>b§VRCAN/1/40§Q§483</t>
+  </si>
+  <si>
+    <t>b§WSSWM3/1/0§Q§560</t>
+  </si>
+  <si>
+    <t>e§JWBOY/2/80§Q§269</t>
+  </si>
+  <si>
+    <t>e§JWBOY/2/80§Q§268</t>
+  </si>
+  <si>
+    <t>b§JARI1/1/80§Q§169</t>
+  </si>
+  <si>
+    <t>d§CRSOSO/3/40§Q§65</t>
+  </si>
+  <si>
+    <t>c§KVEDG1/1/80§Q§283</t>
+  </si>
+  <si>
+    <t>c§PDVRT1/20§Q§409</t>
+  </si>
+  <si>
+    <t>b|CRSOSO-3-40|Q|76</t>
+  </si>
+  <si>
+    <t>maple/cnt§21</t>
+  </si>
+  <si>
+    <t>a§CWRIC2/X2§Q§84</t>
+  </si>
+  <si>
+    <t>a§MHBUR1/4/20§Q§338</t>
+  </si>
+  <si>
+    <t>d§VSGARO1/1/0§Q§540</t>
+  </si>
+  <si>
+    <t>c§DVGM/20§Q§115</t>
+  </si>
+  <si>
+    <t>maple/cnt§19</t>
+  </si>
+  <si>
+    <t>e§JARI1/1/80§Q§189</t>
+  </si>
+  <si>
+    <t>maple/cnt§20</t>
+  </si>
+  <si>
+    <t>maple/cnt§23</t>
+  </si>
+  <si>
+    <t>e§MSMID1/1/20§Q§602</t>
+  </si>
+  <si>
+    <t>c§MHBUR1/4/20§Q§336</t>
+  </si>
+  <si>
+    <t>b§MHNAT1/2/0§Q§359</t>
+  </si>
+  <si>
+    <t>d§BWPEM1/9/0§Q§18</t>
+  </si>
+  <si>
+    <t>a§MSMID1/1/20§Q§366</t>
+  </si>
+  <si>
+    <t>a§KVEDG1/1/80§Q§273</t>
+  </si>
+  <si>
+    <t>a|CWRIC2-X2|Q|80</t>
+  </si>
+  <si>
+    <t>e§DVGM/20§Q§132</t>
+  </si>
+  <si>
+    <t>b§JBCHY1/1/50§Q§223</t>
+  </si>
+  <si>
+    <t>a§SEBRN/1/20§N§i145</t>
+  </si>
+  <si>
+    <t>c§SMITH1/20§Q§468</t>
+  </si>
+  <si>
+    <t>c§JARI1/1/80§Q§173</t>
+  </si>
+  <si>
+    <t>c§DVGM/20§Q§119</t>
+  </si>
+  <si>
+    <t>a§JWBOY/2/80§Q§251</t>
+  </si>
+  <si>
+    <t>b§VRCAN/1/40§Q§487</t>
+  </si>
+  <si>
+    <t>e§CRSOSO/3/40§Q§54</t>
+  </si>
+  <si>
+    <t>c§SMITH1/20§Q§467</t>
+  </si>
+  <si>
+    <t>b§DVGM/20§Q§113</t>
+  </si>
+  <si>
+    <t>c§MHBUR1/4/20§Q§340</t>
+  </si>
+  <si>
+    <t>d§RULEB1/20§N§426</t>
+  </si>
+  <si>
+    <t>c§CWRIC2/X2§Q§95</t>
+  </si>
+  <si>
+    <t>d§JARI1/1/80§Q§179</t>
+  </si>
+  <si>
+    <t>a§DVGM/20§Q§102</t>
+  </si>
+  <si>
+    <t>e§JKFRS1/6/0§V§i122</t>
+  </si>
+  <si>
+    <t>c§NSLJU1/4/0§V§i141</t>
+  </si>
+  <si>
+    <t>e§DVGM/20§Q§131</t>
+  </si>
+  <si>
+    <t>c§JARI1/1/80§Q§177</t>
+  </si>
+  <si>
+    <t>b§SMAKC1/B§N§439</t>
+  </si>
+  <si>
+    <t>d§VSGARO1/1/0§Q§543</t>
+  </si>
+  <si>
+    <t>d§KVEDG1/1/80§Q§296</t>
+  </si>
+  <si>
+    <t>d§SMAKC1/B§N§442</t>
+  </si>
+  <si>
+    <t>d§VRPET2/3/20§Q§526</t>
+  </si>
+  <si>
+    <t>c§JBCHY1/1/50§Q§235</t>
+  </si>
+  <si>
+    <t>a§SEBRN/1/20§N§i147</t>
+  </si>
+  <si>
+    <t>b§PDVRT1/20§Q§406</t>
+  </si>
+  <si>
+    <t>c§MHBUR1/4/20§Q§349</t>
+  </si>
+  <si>
+    <t>b§KVEDG1/1/80§Q§281</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -822,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE9D37E-007A-E94D-8E3B-6BFE43886E1F}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E266"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="H193" sqref="H193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3037,7 +3367,1660 @@
         <v>145</v>
       </c>
     </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>146</v>
+      </c>
+      <c r="B152">
+        <v>15.05</v>
+      </c>
+      <c r="C152" t="s">
+        <v>25</v>
+      </c>
+      <c r="E152" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>147</v>
+      </c>
+      <c r="B153">
+        <v>15.37</v>
+      </c>
+      <c r="C153" t="s">
+        <v>25</v>
+      </c>
+      <c r="E153" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>148</v>
+      </c>
+      <c r="B154">
+        <v>15.3</v>
+      </c>
+      <c r="C154" t="s">
+        <v>25</v>
+      </c>
+      <c r="E154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>149</v>
+      </c>
+      <c r="B155">
+        <v>14.33</v>
+      </c>
+      <c r="C155" t="s">
+        <v>25</v>
+      </c>
+      <c r="E155" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156">
+        <v>14.48</v>
+      </c>
+      <c r="C156" t="s">
+        <v>25</v>
+      </c>
+      <c r="E156" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" t="s">
+        <v>151</v>
+      </c>
+      <c r="B157">
+        <v>16.13</v>
+      </c>
+      <c r="C157" t="s">
+        <v>25</v>
+      </c>
+      <c r="E157" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>152</v>
+      </c>
+      <c r="B158">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="C158" t="s">
+        <v>25</v>
+      </c>
+      <c r="E158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>153</v>
+      </c>
+      <c r="B159">
+        <v>15.85</v>
+      </c>
+      <c r="C159" t="s">
+        <v>25</v>
+      </c>
+      <c r="E159" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>154</v>
+      </c>
+      <c r="B160">
+        <v>15.12</v>
+      </c>
+      <c r="C160" t="s">
+        <v>25</v>
+      </c>
+      <c r="E160" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>155</v>
+      </c>
+      <c r="B161">
+        <v>15.43</v>
+      </c>
+      <c r="C161" t="s">
+        <v>25</v>
+      </c>
+      <c r="E161" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>156</v>
+      </c>
+      <c r="B162">
+        <v>15.44</v>
+      </c>
+      <c r="C162" t="s">
+        <v>25</v>
+      </c>
+      <c r="E162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>157</v>
+      </c>
+      <c r="B163">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="C163" t="s">
+        <v>25</v>
+      </c>
+      <c r="E163" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>158</v>
+      </c>
+      <c r="B164">
+        <v>17.3</v>
+      </c>
+      <c r="C164" t="s">
+        <v>25</v>
+      </c>
+      <c r="E164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>159</v>
+      </c>
+      <c r="B165">
+        <v>15.1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>25</v>
+      </c>
+      <c r="E165" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>160</v>
+      </c>
+      <c r="B166">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="C166" t="s">
+        <v>25</v>
+      </c>
+      <c r="D166" t="s">
+        <v>4</v>
+      </c>
+      <c r="E166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>160</v>
+      </c>
+      <c r="B167">
+        <v>6.22</v>
+      </c>
+      <c r="C167" t="s">
+        <v>4</v>
+      </c>
+      <c r="D167" t="s">
+        <v>4</v>
+      </c>
+      <c r="E167" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>161</v>
+      </c>
+      <c r="B168">
+        <v>14.46</v>
+      </c>
+      <c r="C168" t="s">
+        <v>25</v>
+      </c>
+      <c r="E168" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>162</v>
+      </c>
+      <c r="B169">
+        <v>14.64</v>
+      </c>
+      <c r="C169" t="s">
+        <v>25</v>
+      </c>
+      <c r="E169" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>163</v>
+      </c>
+      <c r="B170">
+        <v>15.04</v>
+      </c>
+      <c r="C170" t="s">
+        <v>25</v>
+      </c>
+      <c r="E170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" t="s">
+        <v>164</v>
+      </c>
+      <c r="B171">
+        <v>14.45</v>
+      </c>
+      <c r="C171" t="s">
+        <v>25</v>
+      </c>
+      <c r="E171" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" t="s">
+        <v>165</v>
+      </c>
+      <c r="B172">
+        <v>6.33</v>
+      </c>
+      <c r="C172" t="s">
+        <v>4</v>
+      </c>
+      <c r="E172" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" t="s">
+        <v>166</v>
+      </c>
+      <c r="B173">
+        <v>6.6</v>
+      </c>
+      <c r="C173" t="s">
+        <v>4</v>
+      </c>
+      <c r="E173" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" t="s">
+        <v>167</v>
+      </c>
+      <c r="B174">
+        <v>6.57</v>
+      </c>
+      <c r="C174" t="s">
+        <v>4</v>
+      </c>
+      <c r="E174" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>168</v>
+      </c>
+      <c r="B175">
+        <v>7.37</v>
+      </c>
+      <c r="C175" t="s">
+        <v>4</v>
+      </c>
+      <c r="E175" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>169</v>
+      </c>
+      <c r="B176">
+        <v>7.17</v>
+      </c>
+      <c r="C176" t="s">
+        <v>4</v>
+      </c>
+      <c r="E176" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>170</v>
+      </c>
+      <c r="B177">
+        <v>5.72</v>
+      </c>
+      <c r="C177" t="s">
+        <v>4</v>
+      </c>
+      <c r="E177" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>171</v>
+      </c>
+      <c r="B178">
+        <v>6.12</v>
+      </c>
+      <c r="C178" t="s">
+        <v>4</v>
+      </c>
+      <c r="E178" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>172</v>
+      </c>
+      <c r="B179">
+        <v>6.33</v>
+      </c>
+      <c r="C179" t="s">
+        <v>4</v>
+      </c>
+      <c r="E179" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>173</v>
+      </c>
+      <c r="B180">
+        <v>6.75</v>
+      </c>
+      <c r="C180" t="s">
+        <v>4</v>
+      </c>
+      <c r="E180" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>174</v>
+      </c>
+      <c r="B181">
+        <v>6.9</v>
+      </c>
+      <c r="C181" t="s">
+        <v>4</v>
+      </c>
+      <c r="E181" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" t="s">
+        <v>175</v>
+      </c>
+      <c r="B182">
+        <v>6.13</v>
+      </c>
+      <c r="C182" t="s">
+        <v>4</v>
+      </c>
+      <c r="E182" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" t="s">
+        <v>176</v>
+      </c>
+      <c r="B183">
+        <v>6.79</v>
+      </c>
+      <c r="C183" t="s">
+        <v>4</v>
+      </c>
+      <c r="E183" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" t="s">
+        <v>177</v>
+      </c>
+      <c r="B184">
+        <v>6.59</v>
+      </c>
+      <c r="C184" t="s">
+        <v>4</v>
+      </c>
+      <c r="E184" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" t="s">
+        <v>178</v>
+      </c>
+      <c r="B185">
+        <v>6.14</v>
+      </c>
+      <c r="C185" t="s">
+        <v>4</v>
+      </c>
+      <c r="E185" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" t="s">
+        <v>179</v>
+      </c>
+      <c r="B186">
+        <v>6.04</v>
+      </c>
+      <c r="C186" t="s">
+        <v>4</v>
+      </c>
+      <c r="E186" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" t="s">
+        <v>180</v>
+      </c>
+      <c r="B187">
+        <v>6.21</v>
+      </c>
+      <c r="C187" t="s">
+        <v>4</v>
+      </c>
+      <c r="E187" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" t="s">
+        <v>181</v>
+      </c>
+      <c r="B188">
+        <v>6.06</v>
+      </c>
+      <c r="C188" t="s">
+        <v>4</v>
+      </c>
+      <c r="E188" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" t="s">
+        <v>182</v>
+      </c>
+      <c r="B189">
+        <v>6.21</v>
+      </c>
+      <c r="C189" t="s">
+        <v>4</v>
+      </c>
+      <c r="E189" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" t="s">
+        <v>183</v>
+      </c>
+      <c r="B190">
+        <v>6.38</v>
+      </c>
+      <c r="C190" t="s">
+        <v>4</v>
+      </c>
+      <c r="E190" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" t="s">
+        <v>184</v>
+      </c>
+      <c r="B191">
+        <v>6.1</v>
+      </c>
+      <c r="C191" t="s">
+        <v>4</v>
+      </c>
+      <c r="E191" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" t="s">
+        <v>185</v>
+      </c>
+      <c r="B192">
+        <v>6.45</v>
+      </c>
+      <c r="C192" t="s">
+        <v>4</v>
+      </c>
+      <c r="E192" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" t="s">
+        <v>186</v>
+      </c>
+      <c r="B193">
+        <v>6.56</v>
+      </c>
+      <c r="C193" t="s">
+        <v>4</v>
+      </c>
+      <c r="E193" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" t="s">
+        <v>187</v>
+      </c>
+      <c r="B194">
+        <v>6.33</v>
+      </c>
+      <c r="C194" t="s">
+        <v>4</v>
+      </c>
+      <c r="E194" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" t="s">
+        <v>188</v>
+      </c>
+      <c r="B195">
+        <v>6.48</v>
+      </c>
+      <c r="C195" t="s">
+        <v>4</v>
+      </c>
+      <c r="E195" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" t="s">
+        <v>189</v>
+      </c>
+      <c r="B196">
+        <v>6.28</v>
+      </c>
+      <c r="C196" t="s">
+        <v>4</v>
+      </c>
+      <c r="E196" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" t="s">
+        <v>190</v>
+      </c>
+      <c r="B197">
+        <v>6.11</v>
+      </c>
+      <c r="C197" t="s">
+        <v>4</v>
+      </c>
+      <c r="E197" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" t="s">
+        <v>191</v>
+      </c>
+      <c r="B198">
+        <v>5.95</v>
+      </c>
+      <c r="C198" t="s">
+        <v>4</v>
+      </c>
+      <c r="E198" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" t="s">
+        <v>192</v>
+      </c>
+      <c r="B199">
+        <v>6.52</v>
+      </c>
+      <c r="C199" t="s">
+        <v>4</v>
+      </c>
+      <c r="E199" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" t="s">
+        <v>193</v>
+      </c>
+      <c r="B200">
+        <v>6.38</v>
+      </c>
+      <c r="C200" t="s">
+        <v>4</v>
+      </c>
+      <c r="E200" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" t="s">
+        <v>194</v>
+      </c>
+      <c r="B201">
+        <v>5.96</v>
+      </c>
+      <c r="C201" t="s">
+        <v>4</v>
+      </c>
+      <c r="E201" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" t="s">
+        <v>195</v>
+      </c>
+      <c r="B202">
+        <v>6.89</v>
+      </c>
+      <c r="C202" t="s">
+        <v>4</v>
+      </c>
+      <c r="E202" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" t="s">
+        <v>196</v>
+      </c>
+      <c r="B203">
+        <v>6.99</v>
+      </c>
+      <c r="C203" t="s">
+        <v>4</v>
+      </c>
+      <c r="E203" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" t="s">
+        <v>197</v>
+      </c>
+      <c r="B204">
+        <v>6.39</v>
+      </c>
+      <c r="C204" t="s">
+        <v>4</v>
+      </c>
+      <c r="E204" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" t="s">
+        <v>198</v>
+      </c>
+      <c r="B205">
+        <v>6.36</v>
+      </c>
+      <c r="C205" t="s">
+        <v>4</v>
+      </c>
+      <c r="E205" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" t="s">
+        <v>199</v>
+      </c>
+      <c r="B206">
+        <v>6.33</v>
+      </c>
+      <c r="C206" t="s">
+        <v>4</v>
+      </c>
+      <c r="E206" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" t="s">
+        <v>200</v>
+      </c>
+      <c r="B207">
+        <v>6.12</v>
+      </c>
+      <c r="C207" t="s">
+        <v>4</v>
+      </c>
+      <c r="E207" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" t="s">
+        <v>201</v>
+      </c>
+      <c r="B208">
+        <v>6.4</v>
+      </c>
+      <c r="C208" t="s">
+        <v>4</v>
+      </c>
+      <c r="E208" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" t="s">
+        <v>202</v>
+      </c>
+      <c r="B209">
+        <v>6.33</v>
+      </c>
+      <c r="C209" t="s">
+        <v>4</v>
+      </c>
+      <c r="E209" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" t="s">
+        <v>203</v>
+      </c>
+      <c r="B210">
+        <v>6.66</v>
+      </c>
+      <c r="C210" t="s">
+        <v>4</v>
+      </c>
+      <c r="E210" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" t="s">
+        <v>204</v>
+      </c>
+      <c r="B211">
+        <v>6.44</v>
+      </c>
+      <c r="C211" t="s">
+        <v>4</v>
+      </c>
+      <c r="E211" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" t="s">
+        <v>205</v>
+      </c>
+      <c r="B212">
+        <v>7.6</v>
+      </c>
+      <c r="C212" t="s">
+        <v>4</v>
+      </c>
+      <c r="E212" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" t="s">
+        <v>206</v>
+      </c>
+      <c r="B213">
+        <v>6.42</v>
+      </c>
+      <c r="C213" t="s">
+        <v>4</v>
+      </c>
+      <c r="E213" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" t="s">
+        <v>207</v>
+      </c>
+      <c r="B214">
+        <v>6.3</v>
+      </c>
+      <c r="C214" t="s">
+        <v>4</v>
+      </c>
+      <c r="E214" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" t="s">
+        <v>208</v>
+      </c>
+      <c r="B215">
+        <v>6.42</v>
+      </c>
+      <c r="C215" t="s">
+        <v>4</v>
+      </c>
+      <c r="E215" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" t="s">
+        <v>209</v>
+      </c>
+      <c r="B216">
+        <v>5.99</v>
+      </c>
+      <c r="C216" t="s">
+        <v>4</v>
+      </c>
+      <c r="E216" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" t="s">
+        <v>210</v>
+      </c>
+      <c r="B217">
+        <v>6.37</v>
+      </c>
+      <c r="C217" t="s">
+        <v>4</v>
+      </c>
+      <c r="E217" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" t="s">
+        <v>211</v>
+      </c>
+      <c r="B218">
+        <v>7.21</v>
+      </c>
+      <c r="C218" t="s">
+        <v>4</v>
+      </c>
+      <c r="E218" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" t="s">
+        <v>212</v>
+      </c>
+      <c r="B219">
+        <v>6.33</v>
+      </c>
+      <c r="C219" t="s">
+        <v>4</v>
+      </c>
+      <c r="E219" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" t="s">
+        <v>213</v>
+      </c>
+      <c r="B220">
+        <v>6.35</v>
+      </c>
+      <c r="C220" t="s">
+        <v>4</v>
+      </c>
+      <c r="E220" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" t="s">
+        <v>214</v>
+      </c>
+      <c r="B221">
+        <v>6.39</v>
+      </c>
+      <c r="C221" t="s">
+        <v>4</v>
+      </c>
+      <c r="E221" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" t="s">
+        <v>215</v>
+      </c>
+      <c r="B222">
+        <v>7.34</v>
+      </c>
+      <c r="C222" t="s">
+        <v>4</v>
+      </c>
+      <c r="E222" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" t="s">
+        <v>216</v>
+      </c>
+      <c r="B223">
+        <v>7.08</v>
+      </c>
+      <c r="C223" t="s">
+        <v>4</v>
+      </c>
+      <c r="E223" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" t="s">
+        <v>217</v>
+      </c>
+      <c r="B224">
+        <v>6.73</v>
+      </c>
+      <c r="C224" t="s">
+        <v>4</v>
+      </c>
+      <c r="E224" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" t="s">
+        <v>218</v>
+      </c>
+      <c r="B225">
+        <v>6.67</v>
+      </c>
+      <c r="C225" t="s">
+        <v>4</v>
+      </c>
+      <c r="E225" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" t="s">
+        <v>219</v>
+      </c>
+      <c r="B226">
+        <v>6.5</v>
+      </c>
+      <c r="C226" t="s">
+        <v>4</v>
+      </c>
+      <c r="E226" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" t="s">
+        <v>220</v>
+      </c>
+      <c r="B227">
+        <v>9.01</v>
+      </c>
+      <c r="C227" t="s">
+        <v>25</v>
+      </c>
+      <c r="E227" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" t="s">
+        <v>221</v>
+      </c>
+      <c r="B228">
+        <v>9.92</v>
+      </c>
+      <c r="C228" t="s">
+        <v>25</v>
+      </c>
+      <c r="E228" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" t="s">
+        <v>222</v>
+      </c>
+      <c r="B229">
+        <v>10.01</v>
+      </c>
+      <c r="C229" t="s">
+        <v>25</v>
+      </c>
+      <c r="E229" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" t="s">
+        <v>223</v>
+      </c>
+      <c r="B230">
+        <v>8.64</v>
+      </c>
+      <c r="C230" t="s">
+        <v>25</v>
+      </c>
+      <c r="D230" t="s">
+        <v>4</v>
+      </c>
+      <c r="E230" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" t="s">
+        <v>223</v>
+      </c>
+      <c r="B231">
+        <v>6.46</v>
+      </c>
+      <c r="C231" t="s">
+        <v>4</v>
+      </c>
+      <c r="D231" t="s">
+        <v>4</v>
+      </c>
+      <c r="E231" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" t="s">
+        <v>224</v>
+      </c>
+      <c r="B232">
+        <v>18.96</v>
+      </c>
+      <c r="C232" t="s">
+        <v>25</v>
+      </c>
+      <c r="E232" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" t="s">
+        <v>225</v>
+      </c>
+      <c r="B233">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="C233" t="s">
+        <v>25</v>
+      </c>
+      <c r="E233" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" t="s">
+        <v>226</v>
+      </c>
+      <c r="B234">
+        <v>19.37</v>
+      </c>
+      <c r="C234" t="s">
+        <v>25</v>
+      </c>
+      <c r="E234" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" t="s">
+        <v>227</v>
+      </c>
+      <c r="B235">
+        <v>9.51</v>
+      </c>
+      <c r="C235" t="s">
+        <v>25</v>
+      </c>
+      <c r="D235" t="s">
+        <v>4</v>
+      </c>
+      <c r="E235" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" t="s">
+        <v>227</v>
+      </c>
+      <c r="B236">
+        <v>6.61</v>
+      </c>
+      <c r="C236" t="s">
+        <v>4</v>
+      </c>
+      <c r="D236" t="s">
+        <v>4</v>
+      </c>
+      <c r="E236" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" t="s">
+        <v>228</v>
+      </c>
+      <c r="B237">
+        <v>12.25</v>
+      </c>
+      <c r="C237" t="s">
+        <v>25</v>
+      </c>
+      <c r="E237" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" t="s">
+        <v>229</v>
+      </c>
+      <c r="B238">
+        <v>9.19</v>
+      </c>
+      <c r="C238" t="s">
+        <v>25</v>
+      </c>
+      <c r="E238" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239" t="s">
+        <v>230</v>
+      </c>
+      <c r="B239">
+        <v>8.6</v>
+      </c>
+      <c r="C239" t="s">
+        <v>25</v>
+      </c>
+      <c r="E239" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" t="s">
+        <v>231</v>
+      </c>
+      <c r="B240">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="C240" t="s">
+        <v>25</v>
+      </c>
+      <c r="D240" t="s">
+        <v>4</v>
+      </c>
+      <c r="E240" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" t="s">
+        <v>231</v>
+      </c>
+      <c r="B241">
+        <v>5.98</v>
+      </c>
+      <c r="C241" t="s">
+        <v>4</v>
+      </c>
+      <c r="D241" t="s">
+        <v>4</v>
+      </c>
+      <c r="E241" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" t="s">
+        <v>232</v>
+      </c>
+      <c r="B242">
+        <v>8.99</v>
+      </c>
+      <c r="C242" t="s">
+        <v>25</v>
+      </c>
+      <c r="E242" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" t="s">
+        <v>233</v>
+      </c>
+      <c r="B243">
+        <v>10.3</v>
+      </c>
+      <c r="C243" t="s">
+        <v>25</v>
+      </c>
+      <c r="E243" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" t="s">
+        <v>234</v>
+      </c>
+      <c r="B244">
+        <v>10.6</v>
+      </c>
+      <c r="C244" t="s">
+        <v>25</v>
+      </c>
+      <c r="E244" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245" t="s">
+        <v>235</v>
+      </c>
+      <c r="B245">
+        <v>9.01</v>
+      </c>
+      <c r="C245" t="s">
+        <v>25</v>
+      </c>
+      <c r="D245" t="s">
+        <v>4</v>
+      </c>
+      <c r="E245" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246" t="s">
+        <v>235</v>
+      </c>
+      <c r="B246">
+        <v>6.28</v>
+      </c>
+      <c r="C246" t="s">
+        <v>4</v>
+      </c>
+      <c r="D246" t="s">
+        <v>4</v>
+      </c>
+      <c r="E246" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" t="s">
+        <v>236</v>
+      </c>
+      <c r="B247">
+        <v>12.51</v>
+      </c>
+      <c r="C247" t="s">
+        <v>25</v>
+      </c>
+      <c r="E247" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" t="s">
+        <v>237</v>
+      </c>
+      <c r="B248">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="C248" t="s">
+        <v>25</v>
+      </c>
+      <c r="E248" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" t="s">
+        <v>238</v>
+      </c>
+      <c r="B249">
+        <v>9.07</v>
+      </c>
+      <c r="C249" t="s">
+        <v>25</v>
+      </c>
+      <c r="E249" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" t="s">
+        <v>239</v>
+      </c>
+      <c r="B250">
+        <v>9.6</v>
+      </c>
+      <c r="C250" t="s">
+        <v>25</v>
+      </c>
+      <c r="E250" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" t="s">
+        <v>240</v>
+      </c>
+      <c r="B251">
+        <v>14.47</v>
+      </c>
+      <c r="C251" t="s">
+        <v>25</v>
+      </c>
+      <c r="E251" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" t="s">
+        <v>241</v>
+      </c>
+      <c r="B252">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="C252" t="s">
+        <v>25</v>
+      </c>
+      <c r="E252" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5">
+      <c r="A253" t="s">
+        <v>242</v>
+      </c>
+      <c r="B253">
+        <v>17.829999999999998</v>
+      </c>
+      <c r="C253" t="s">
+        <v>25</v>
+      </c>
+      <c r="E253" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
+      <c r="A254" t="s">
+        <v>243</v>
+      </c>
+      <c r="B254">
+        <v>9.75</v>
+      </c>
+      <c r="C254" t="s">
+        <v>25</v>
+      </c>
+      <c r="E254" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5">
+      <c r="A255" t="s">
+        <v>244</v>
+      </c>
+      <c r="B255">
+        <v>11.62</v>
+      </c>
+      <c r="C255" t="s">
+        <v>25</v>
+      </c>
+      <c r="D255" t="s">
+        <v>4</v>
+      </c>
+      <c r="E255" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
+      <c r="A256" t="s">
+        <v>244</v>
+      </c>
+      <c r="B256">
+        <v>6.24</v>
+      </c>
+      <c r="C256" t="s">
+        <v>4</v>
+      </c>
+      <c r="D256" t="s">
+        <v>4</v>
+      </c>
+      <c r="E256" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5">
+      <c r="A257" t="s">
+        <v>245</v>
+      </c>
+      <c r="B257">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="C257" t="s">
+        <v>25</v>
+      </c>
+      <c r="E257" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
+      <c r="A258" t="s">
+        <v>246</v>
+      </c>
+      <c r="B258">
+        <v>9.68</v>
+      </c>
+      <c r="C258" t="s">
+        <v>25</v>
+      </c>
+      <c r="D258" t="s">
+        <v>4</v>
+      </c>
+      <c r="E258" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" t="s">
+        <v>246</v>
+      </c>
+      <c r="B259">
+        <v>6.45</v>
+      </c>
+      <c r="C259" t="s">
+        <v>4</v>
+      </c>
+      <c r="D259" t="s">
+        <v>4</v>
+      </c>
+      <c r="E259" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5">
+      <c r="A260" t="s">
+        <v>247</v>
+      </c>
+      <c r="B260">
+        <v>9.9</v>
+      </c>
+      <c r="C260" t="s">
+        <v>25</v>
+      </c>
+      <c r="E260" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5">
+      <c r="A261" t="s">
+        <v>248</v>
+      </c>
+      <c r="B261">
+        <v>10.1</v>
+      </c>
+      <c r="C261" t="s">
+        <v>25</v>
+      </c>
+      <c r="E261" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5">
+      <c r="A262" t="s">
+        <v>249</v>
+      </c>
+      <c r="B262">
+        <v>10.42</v>
+      </c>
+      <c r="C262" t="s">
+        <v>25</v>
+      </c>
+      <c r="E262" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" t="s">
+        <v>250</v>
+      </c>
+      <c r="B263">
+        <v>12.56</v>
+      </c>
+      <c r="C263" t="s">
+        <v>25</v>
+      </c>
+      <c r="E263" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5">
+      <c r="A264" t="s">
+        <v>251</v>
+      </c>
+      <c r="B264">
+        <v>11.36</v>
+      </c>
+      <c r="C264" t="s">
+        <v>25</v>
+      </c>
+      <c r="E264" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" t="s">
+        <v>252</v>
+      </c>
+      <c r="B265">
+        <v>12.87</v>
+      </c>
+      <c r="C265" t="s">
+        <v>25</v>
+      </c>
+      <c r="E265" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" t="s">
+        <v>253</v>
+      </c>
+      <c r="B266">
+        <v>8.83</v>
+      </c>
+      <c r="C266" t="s">
+        <v>25</v>
+      </c>
+      <c r="E266" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>